<commit_message>
Child and Case functionality left
Most procedures and functions have been coded. What's left are just child procedures and case functionality. And also I haven't touched main yet
</commit_message>
<xml_diff>
--- a/Penilaian Tubes ASD 2018.xlsx
+++ b/Penilaian Tubes ASD 2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANDITYAARIFIANTO\Google Drive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Tubes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9AE1538-0CA2-48FF-A26F-536F8B35FF16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAAE776-2E73-46BC-B6BC-187808B1AB93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{BB18EACF-535A-4B2D-B714-15E04ABCC3B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BB18EACF-535A-4B2D-B714-15E04ABCC3B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,7 +282,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +328,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,73 +408,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,638 +799,647 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>80</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>80</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>100</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="3" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="21">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="21">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="21">
+        <v>5</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="21"/>
+      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="21"/>
+      <c r="G5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="4" t="s">
+      <c r="F6" s="21"/>
+      <c r="G6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7">
-        <v>5</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="22">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7">
-        <v>5</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="22">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="7">
-        <v>5</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="F7" s="22">
+        <v>5</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="H7" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6" t="s">
+      <c r="F8" s="22"/>
+      <c r="G8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="22"/>
+      <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6" t="s">
+      <c r="F9" s="22"/>
+      <c r="G9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="22"/>
+      <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="6" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9" t="s">
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="13">
         <v>3</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="13">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9" t="s">
+    <row r="12" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12">
-        <v>5</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="B13" s="8">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="12">
-        <v>5</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="12">
-        <v>5</v>
-      </c>
-      <c r="G13" s="11" t="s">
+      <c r="F13" s="8">
+        <v>5</v>
+      </c>
+      <c r="G13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="H13" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="8">
         <v>2</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="8">
         <v>2</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="8">
         <v>2</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="12">
-        <v>5</v>
-      </c>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="8">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="12">
-        <v>5</v>
-      </c>
-      <c r="E15" s="11" t="s">
+      <c r="D15" s="8">
+        <v>5</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="12">
-        <v>5</v>
-      </c>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="8">
+        <v>5</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="H15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="8">
         <v>2</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="8">
         <v>4</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="8">
         <v>2</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="8">
         <v>4</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="11" t="s">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="8">
         <v>6</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="8">
         <v>2</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="8">
         <v>2</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="8">
         <v>4</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="8">
         <v>2</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="11" t="s">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="8">
         <v>6</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="8">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="8">
         <v>4</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="8">
         <v>4</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="12">
-        <v>5</v>
-      </c>
-      <c r="G20" s="11" t="s">
+      <c r="F20" s="8">
+        <v>5</v>
+      </c>
+      <c r="G20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="H20" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="8">
         <v>4</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="8">
         <v>4</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="8">
         <v>4</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="8">
         <v>10</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="8">
         <v>12</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="8">
         <v>14</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="8">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="8">
         <v>10</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="8">
         <v>12</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="8">
         <v>14</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="8">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+    <row r="24" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="10">
         <v>10</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="10">
         <v>10</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="10">
         <v>10</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+    <row r="25" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="10">
         <v>10</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="10">
         <v>10</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="10">
         <v>10</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="14">
+      <c r="H25" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="21"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="C29" s="19"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="21"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="C30" s="19"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="21"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
+      <c r="C31" s="19"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="22"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="H3:H6"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B32:C34"/>
@@ -1420,15 +1447,6 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="H7:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
functionality and main left
every standard function has been coded. will work on main next and functionality last
</commit_message>
<xml_diff>
--- a/Penilaian Tubes ASD 2018.xlsx
+++ b/Penilaian Tubes ASD 2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Tubes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAAE776-2E73-46BC-B6BC-187808B1AB93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C9C2C8-9ED3-4AA0-9B9D-0F7DC87BE6EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BB18EACF-535A-4B2D-B714-15E04ABCC3B2}"/>
   </bookViews>
@@ -282,7 +282,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,12 +334,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -446,6 +440,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -466,21 +472,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,8 +790,8 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,16 +808,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -858,25 +849,25 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="16">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="16">
         <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="21">
-        <v>5</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="21">
+      <c r="F3" s="16">
+        <v>5</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="16">
         <v>5</v>
       </c>
     </row>
@@ -884,79 +875,79 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="23" t="s">
+      <c r="F4" s="16"/>
+      <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="21"/>
+      <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="23" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="21"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="23" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="14">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="14">
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="22">
-        <v>5</v>
-      </c>
-      <c r="G7" s="23" t="s">
+      <c r="F7" s="14">
+        <v>5</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="14">
         <v>5</v>
       </c>
     </row>
@@ -964,55 +955,55 @@
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="22"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="24" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="24" t="s">
+      <c r="F9" s="14"/>
+      <c r="G9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="22"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
@@ -1022,13 +1013,13 @@
       <c r="E11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="17">
         <v>3</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="17">
         <v>3</v>
       </c>
     </row>
@@ -1040,11 +1031,11 @@
       <c r="E12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="23" t="s">
+      <c r="F12" s="17"/>
+      <c r="G12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="17"/>
     </row>
     <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
@@ -1065,7 +1056,7 @@
       <c r="F13" s="8">
         <v>5</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H13" s="8">
@@ -1091,7 +1082,7 @@
       <c r="F14" s="8">
         <v>2</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="13" t="s">
         <v>13</v>
       </c>
       <c r="H14" s="8">
@@ -1117,7 +1108,7 @@
       <c r="F15" s="8">
         <v>5</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="8">
@@ -1143,7 +1134,7 @@
       <c r="F16" s="8">
         <v>2</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="8">
@@ -1165,7 +1156,7 @@
       <c r="F17" s="8">
         <v>6</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="13" t="s">
         <v>19</v>
       </c>
       <c r="H17" s="8">
@@ -1191,7 +1182,7 @@
       <c r="F18" s="8">
         <v>4</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H18" s="8">
@@ -1213,7 +1204,7 @@
       <c r="F19" s="8">
         <v>6</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="13" t="s">
         <v>26</v>
       </c>
       <c r="H19" s="8">
@@ -1239,7 +1230,7 @@
       <c r="F20" s="8">
         <v>5</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="13" t="s">
         <v>27</v>
       </c>
       <c r="H20" s="8">
@@ -1265,7 +1256,7 @@
       <c r="F21" s="8">
         <v>4</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="13" t="s">
         <v>28</v>
       </c>
       <c r="H21" s="8">
@@ -1291,7 +1282,7 @@
       <c r="F22" s="8">
         <v>14</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="13" t="s">
         <v>32</v>
       </c>
       <c r="H22" s="8">
@@ -1317,7 +1308,7 @@
       <c r="F23" s="8">
         <v>14</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="13" t="s">
         <v>35</v>
       </c>
       <c r="H23" s="8">
@@ -1377,60 +1368,67 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="23"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="19"/>
+      <c r="C30" s="23"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="19"/>
+      <c r="C31" s="23"/>
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="14"/>
+      <c r="C32" s="18"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="12"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B32:C34"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="F7:F10"/>
@@ -1440,13 +1438,6 @@
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="H3:H6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B32:C34"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>